<commit_message>
Small error handling update
</commit_message>
<xml_diff>
--- a/excel/debugging.xlsx
+++ b/excel/debugging.xlsx
@@ -5,12 +5,12 @@
   <workbookPr hidePivotFieldList="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\graha\OneDrive\Documents\GitHub\application_tracker\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\graha\OneDrive\Documents\GitHub\application_tracker\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A8F5C78-822E-4C4D-BA06-BE12FF80EEEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90A9F429-AB32-4C55-A972-661B00A41998}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="18940" yWindow="6940" windowWidth="19440" windowHeight="13720" xr2:uid="{85E7A6A4-6F22-48D9-815F-FC03736B7AC4}"/>
+    <workbookView xWindow="1140" yWindow="1140" windowWidth="19440" windowHeight="13720" xr2:uid="{85E7A6A4-6F22-48D9-815F-FC03736B7AC4}"/>
   </bookViews>
   <sheets>
     <sheet name="Tracker" sheetId="1" r:id="rId1"/>
@@ -1644,11 +1644,11 @@
       </c>
       <c r="G2">
         <f t="shared" ref="G2:G33" ca="1" si="0">ROUND(RAND()*60+40,0)</f>
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="H2">
         <f t="shared" ref="H2:H33" ca="1" si="1">ROUND(RAND()*40+90,0)</f>
-        <v>101</v>
+        <v>116</v>
       </c>
       <c r="I2" s="1" t="s">
         <v>231</v>
@@ -1696,11 +1696,11 @@
       </c>
       <c r="G3">
         <f t="shared" ca="1" si="0"/>
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="H3">
         <f t="shared" ca="1" si="1"/>
-        <v>124</v>
+        <v>112</v>
       </c>
       <c r="I3" s="1" t="s">
         <v>228</v>
@@ -1748,11 +1748,11 @@
       </c>
       <c r="G4">
         <f t="shared" ca="1" si="0"/>
-        <v>45</v>
+        <v>73</v>
       </c>
       <c r="H4">
         <f t="shared" ca="1" si="1"/>
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="I4" s="1" t="s">
         <v>229</v>
@@ -1795,11 +1795,11 @@
       </c>
       <c r="G5">
         <f t="shared" ca="1" si="0"/>
-        <v>85</v>
+        <v>73</v>
       </c>
       <c r="H5">
         <f t="shared" ca="1" si="1"/>
-        <v>123</v>
+        <v>115</v>
       </c>
       <c r="I5" s="1" t="s">
         <v>230</v>
@@ -1844,11 +1844,11 @@
       </c>
       <c r="G6">
         <f t="shared" ca="1" si="0"/>
-        <v>96</v>
+        <v>79</v>
       </c>
       <c r="H6">
         <f t="shared" ca="1" si="1"/>
-        <v>108</v>
+        <v>129</v>
       </c>
       <c r="I6" s="1" t="s">
         <v>227</v>
@@ -1896,11 +1896,11 @@
       </c>
       <c r="G7">
         <f t="shared" ca="1" si="0"/>
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="H7">
         <f t="shared" ca="1" si="1"/>
-        <v>119</v>
+        <v>93</v>
       </c>
       <c r="I7" s="1" t="s">
         <v>227</v>
@@ -1945,11 +1945,11 @@
       </c>
       <c r="G8">
         <f t="shared" ca="1" si="0"/>
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="H8">
         <f t="shared" ca="1" si="1"/>
-        <v>118</v>
+        <v>98</v>
       </c>
       <c r="I8" s="1" t="s">
         <v>228</v>
@@ -1995,11 +1995,11 @@
       </c>
       <c r="G9">
         <f t="shared" ca="1" si="0"/>
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="H9">
         <f t="shared" ca="1" si="1"/>
-        <v>120</v>
+        <v>92</v>
       </c>
       <c r="I9" s="1" t="s">
         <v>229</v>
@@ -2047,11 +2047,11 @@
       </c>
       <c r="G10">
         <f t="shared" ca="1" si="0"/>
-        <v>69</v>
+        <v>48</v>
       </c>
       <c r="H10">
         <f t="shared" ca="1" si="1"/>
-        <v>113</v>
+        <v>126</v>
       </c>
       <c r="I10" s="1" t="s">
         <v>228</v>
@@ -2094,11 +2094,11 @@
       </c>
       <c r="G11">
         <f t="shared" ca="1" si="0"/>
-        <v>99</v>
+        <v>62</v>
       </c>
       <c r="H11">
         <f t="shared" ca="1" si="1"/>
-        <v>114</v>
+        <v>94</v>
       </c>
       <c r="I11" s="1" t="s">
         <v>229</v>
@@ -2143,11 +2143,11 @@
       </c>
       <c r="G12">
         <f t="shared" ca="1" si="0"/>
-        <v>47</v>
+        <v>87</v>
       </c>
       <c r="H12">
         <f t="shared" ca="1" si="1"/>
-        <v>120</v>
+        <v>102</v>
       </c>
       <c r="I12" s="1" t="s">
         <v>229</v>
@@ -2195,11 +2195,11 @@
       </c>
       <c r="G13">
         <f t="shared" ca="1" si="0"/>
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="H13">
         <f t="shared" ca="1" si="1"/>
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="I13" s="1" t="s">
         <v>228</v>
@@ -2244,11 +2244,11 @@
       </c>
       <c r="G14">
         <f t="shared" ca="1" si="0"/>
-        <v>46</v>
+        <v>100</v>
       </c>
       <c r="H14">
         <f t="shared" ca="1" si="1"/>
-        <v>96</v>
+        <v>101</v>
       </c>
       <c r="I14" s="1" t="s">
         <v>229</v>
@@ -2293,11 +2293,11 @@
       </c>
       <c r="G15">
         <f t="shared" ca="1" si="0"/>
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="H15">
         <f t="shared" ca="1" si="1"/>
-        <v>105</v>
+        <v>123</v>
       </c>
       <c r="I15" s="1" t="s">
         <v>228</v>
@@ -2339,11 +2339,11 @@
       </c>
       <c r="G16">
         <f t="shared" ca="1" si="0"/>
-        <v>70</v>
+        <v>88</v>
       </c>
       <c r="H16">
         <f t="shared" ca="1" si="1"/>
-        <v>122</v>
+        <v>128</v>
       </c>
       <c r="I16" s="1" t="s">
         <v>230</v>
@@ -2385,11 +2385,11 @@
       </c>
       <c r="G17">
         <f t="shared" ca="1" si="0"/>
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="H17">
         <f t="shared" ca="1" si="1"/>
-        <v>116</v>
+        <v>126</v>
       </c>
       <c r="I17" s="1" t="s">
         <v>228</v>
@@ -2434,11 +2434,11 @@
       </c>
       <c r="G18">
         <f t="shared" ca="1" si="0"/>
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="H18">
         <f t="shared" ca="1" si="1"/>
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="I18" s="1" t="s">
         <v>229</v>
@@ -2483,11 +2483,11 @@
       </c>
       <c r="G19">
         <f t="shared" ca="1" si="0"/>
-        <v>84</v>
+        <v>45</v>
       </c>
       <c r="H19">
         <f t="shared" ca="1" si="1"/>
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="I19" s="1" t="s">
         <v>228</v>
@@ -2532,11 +2532,11 @@
       </c>
       <c r="G20">
         <f t="shared" ca="1" si="0"/>
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="H20">
         <f t="shared" ca="1" si="1"/>
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="I20" s="1" t="s">
         <v>230</v>
@@ -2581,11 +2581,11 @@
       </c>
       <c r="G21">
         <f t="shared" ca="1" si="0"/>
-        <v>85</v>
+        <v>52</v>
       </c>
       <c r="H21">
         <f t="shared" ca="1" si="1"/>
-        <v>122</v>
+        <v>105</v>
       </c>
       <c r="I21" s="1" t="s">
         <v>230</v>
@@ -2627,11 +2627,11 @@
       </c>
       <c r="G22">
         <f t="shared" ca="1" si="0"/>
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="H22">
         <f t="shared" ca="1" si="1"/>
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="I22" s="1" t="s">
         <v>227</v>
@@ -2676,11 +2676,11 @@
       </c>
       <c r="G23">
         <f t="shared" ca="1" si="0"/>
-        <v>56</v>
+        <v>82</v>
       </c>
       <c r="H23">
         <f t="shared" ca="1" si="1"/>
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="I23" s="1" t="s">
         <v>227</v>
@@ -2725,11 +2725,11 @@
       </c>
       <c r="G24">
         <f t="shared" ca="1" si="0"/>
-        <v>55</v>
+        <v>95</v>
       </c>
       <c r="H24">
         <f t="shared" ca="1" si="1"/>
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="I24" s="1" t="s">
         <v>230</v>
@@ -2777,11 +2777,11 @@
       </c>
       <c r="G25">
         <f t="shared" ca="1" si="0"/>
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="H25">
         <f t="shared" ca="1" si="1"/>
-        <v>90</v>
+        <v>123</v>
       </c>
       <c r="I25" s="1" t="s">
         <v>229</v>
@@ -2826,11 +2826,11 @@
       </c>
       <c r="G26">
         <f t="shared" ca="1" si="0"/>
-        <v>63</v>
+        <v>79</v>
       </c>
       <c r="H26">
         <f t="shared" ca="1" si="1"/>
-        <v>122</v>
+        <v>107</v>
       </c>
       <c r="I26" s="1" t="s">
         <v>229</v>
@@ -2872,11 +2872,11 @@
       </c>
       <c r="G27">
         <f t="shared" ca="1" si="0"/>
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="H27">
         <f t="shared" ca="1" si="1"/>
-        <v>96</v>
+        <v>125</v>
       </c>
       <c r="I27" s="1" t="s">
         <v>230</v>
@@ -2918,11 +2918,11 @@
       </c>
       <c r="G28">
         <f t="shared" ca="1" si="0"/>
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="H28">
         <f t="shared" ca="1" si="1"/>
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="I28" s="1" t="s">
         <v>228</v>
@@ -2967,11 +2967,11 @@
       </c>
       <c r="G29">
         <f t="shared" ca="1" si="0"/>
-        <v>64</v>
+        <v>84</v>
       </c>
       <c r="H29">
         <f t="shared" ca="1" si="1"/>
-        <v>111</v>
+        <v>91</v>
       </c>
       <c r="I29" s="1" t="s">
         <v>229</v>
@@ -3013,11 +3013,11 @@
       </c>
       <c r="G30">
         <f t="shared" ca="1" si="0"/>
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="H30">
         <f t="shared" ca="1" si="1"/>
-        <v>120</v>
+        <v>112</v>
       </c>
       <c r="I30" s="1" t="s">
         <v>228</v>
@@ -3062,11 +3062,11 @@
       </c>
       <c r="G31">
         <f t="shared" ca="1" si="0"/>
-        <v>54</v>
+        <v>69</v>
       </c>
       <c r="H31">
         <f t="shared" ca="1" si="1"/>
-        <v>117</v>
+        <v>122</v>
       </c>
       <c r="I31" s="1" t="s">
         <v>231</v>
@@ -3111,11 +3111,11 @@
       </c>
       <c r="G32">
         <f t="shared" ca="1" si="0"/>
-        <v>73</v>
+        <v>46</v>
       </c>
       <c r="H32">
         <f t="shared" ca="1" si="1"/>
-        <v>98</v>
+        <v>118</v>
       </c>
       <c r="I32" s="1" t="s">
         <v>231</v>
@@ -3158,11 +3158,11 @@
       </c>
       <c r="G33">
         <f t="shared" ca="1" si="0"/>
-        <v>69</v>
+        <v>41</v>
       </c>
       <c r="H33">
         <f t="shared" ca="1" si="1"/>
-        <v>117</v>
+        <v>90</v>
       </c>
       <c r="I33" s="1" t="s">
         <v>230</v>
@@ -3205,11 +3205,11 @@
       </c>
       <c r="G34">
         <f t="shared" ref="G34:G65" ca="1" si="5">ROUND(RAND()*60+40,0)</f>
-        <v>93</v>
+        <v>77</v>
       </c>
       <c r="H34">
         <f t="shared" ref="H34:H65" ca="1" si="6">ROUND(RAND()*40+90,0)</f>
-        <v>99</v>
+        <v>114</v>
       </c>
       <c r="I34" s="1" t="s">
         <v>231</v>
@@ -3251,11 +3251,11 @@
       </c>
       <c r="G35">
         <f t="shared" ca="1" si="5"/>
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="H35">
         <f t="shared" ca="1" si="6"/>
-        <v>96</v>
+        <v>106</v>
       </c>
       <c r="I35" s="1" t="s">
         <v>229</v>
@@ -3303,11 +3303,11 @@
       </c>
       <c r="G36">
         <f t="shared" ca="1" si="5"/>
-        <v>90</v>
+        <v>59</v>
       </c>
       <c r="H36">
         <f t="shared" ca="1" si="6"/>
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="I36" s="1" t="s">
         <v>231</v>
@@ -3350,11 +3350,11 @@
       </c>
       <c r="G37">
         <f t="shared" ca="1" si="5"/>
-        <v>95</v>
+        <v>42</v>
       </c>
       <c r="H37">
         <f t="shared" ca="1" si="6"/>
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="I37" s="1" t="s">
         <v>227</v>
@@ -3397,11 +3397,11 @@
       </c>
       <c r="G38">
         <f t="shared" ca="1" si="5"/>
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="H38">
         <f t="shared" ca="1" si="6"/>
-        <v>105</v>
+        <v>129</v>
       </c>
       <c r="I38" s="1" t="s">
         <v>229</v>
@@ -3443,11 +3443,11 @@
       </c>
       <c r="G39">
         <f t="shared" ca="1" si="5"/>
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="H39">
         <f t="shared" ca="1" si="6"/>
-        <v>117</v>
+        <v>92</v>
       </c>
       <c r="I39" s="1" t="s">
         <v>230</v>
@@ -3490,11 +3490,11 @@
       </c>
       <c r="G40">
         <f t="shared" ca="1" si="5"/>
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="H40">
         <f t="shared" ca="1" si="6"/>
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="I40" s="1" t="s">
         <v>231</v>
@@ -3539,11 +3539,11 @@
       </c>
       <c r="G41">
         <f t="shared" ca="1" si="5"/>
-        <v>44</v>
+        <v>61</v>
       </c>
       <c r="H41">
         <f t="shared" ca="1" si="6"/>
-        <v>104</v>
+        <v>115</v>
       </c>
       <c r="I41" s="1" t="s">
         <v>231</v>
@@ -3585,11 +3585,11 @@
       </c>
       <c r="G42">
         <f t="shared" ca="1" si="5"/>
-        <v>58</v>
+        <v>76</v>
       </c>
       <c r="H42">
         <f t="shared" ca="1" si="6"/>
-        <v>93</v>
+        <v>122</v>
       </c>
       <c r="I42" s="1" t="s">
         <v>229</v>
@@ -3631,11 +3631,11 @@
       </c>
       <c r="G43">
         <f t="shared" ca="1" si="5"/>
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="H43">
         <f t="shared" ca="1" si="6"/>
-        <v>100</v>
+        <v>105</v>
       </c>
       <c r="I43" s="1" t="s">
         <v>231</v>
@@ -3678,11 +3678,11 @@
       </c>
       <c r="G44">
         <f t="shared" ca="1" si="5"/>
-        <v>89</v>
+        <v>61</v>
       </c>
       <c r="H44">
         <f t="shared" ca="1" si="6"/>
-        <v>124</v>
+        <v>108</v>
       </c>
       <c r="I44" s="1" t="s">
         <v>231</v>
@@ -3724,11 +3724,11 @@
       </c>
       <c r="G45">
         <f t="shared" ca="1" si="5"/>
-        <v>50</v>
+        <v>65</v>
       </c>
       <c r="H45">
         <f t="shared" ca="1" si="6"/>
-        <v>125</v>
+        <v>113</v>
       </c>
       <c r="I45" s="1" t="s">
         <v>228</v>
@@ -3770,11 +3770,11 @@
       </c>
       <c r="G46">
         <f t="shared" ca="1" si="5"/>
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="H46">
         <f t="shared" ca="1" si="6"/>
-        <v>122</v>
+        <v>128</v>
       </c>
       <c r="I46" s="1" t="s">
         <v>231</v>
@@ -3822,11 +3822,11 @@
       </c>
       <c r="G47">
         <f t="shared" ca="1" si="5"/>
-        <v>45</v>
+        <v>86</v>
       </c>
       <c r="H47">
         <f t="shared" ca="1" si="6"/>
-        <v>106</v>
+        <v>91</v>
       </c>
       <c r="I47" s="1" t="s">
         <v>227</v>
@@ -3868,11 +3868,11 @@
       </c>
       <c r="G48">
         <f t="shared" ca="1" si="5"/>
-        <v>81</v>
+        <v>93</v>
       </c>
       <c r="H48">
         <f t="shared" ca="1" si="6"/>
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="I48" s="1" t="s">
         <v>229</v>
@@ -3914,11 +3914,11 @@
       </c>
       <c r="G49">
         <f t="shared" ca="1" si="5"/>
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H49">
         <f t="shared" ca="1" si="6"/>
-        <v>126</v>
+        <v>116</v>
       </c>
       <c r="I49" s="1" t="s">
         <v>228</v>
@@ -3963,11 +3963,11 @@
       </c>
       <c r="G50">
         <f t="shared" ca="1" si="5"/>
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="H50">
         <f t="shared" ca="1" si="6"/>
-        <v>99</v>
+        <v>107</v>
       </c>
       <c r="I50" s="1" t="s">
         <v>228</v>
@@ -4010,11 +4010,11 @@
       </c>
       <c r="G51">
         <f t="shared" ca="1" si="5"/>
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="H51">
         <f t="shared" ca="1" si="6"/>
-        <v>109</v>
+        <v>126</v>
       </c>
       <c r="I51" s="1" t="s">
         <v>227</v>
@@ -4056,11 +4056,11 @@
       </c>
       <c r="G52">
         <f t="shared" ca="1" si="5"/>
-        <v>58</v>
+        <v>44</v>
       </c>
       <c r="H52">
         <f t="shared" ca="1" si="6"/>
-        <v>98</v>
+        <v>124</v>
       </c>
       <c r="I52" s="1" t="s">
         <v>229</v>
@@ -4105,11 +4105,11 @@
       </c>
       <c r="G53">
         <f t="shared" ca="1" si="5"/>
-        <v>47</v>
+        <v>98</v>
       </c>
       <c r="H53">
         <f t="shared" ca="1" si="6"/>
-        <v>129</v>
+        <v>95</v>
       </c>
       <c r="I53" s="1" t="s">
         <v>231</v>
@@ -4151,11 +4151,11 @@
       </c>
       <c r="G54">
         <f t="shared" ca="1" si="5"/>
-        <v>71</v>
+        <v>85</v>
       </c>
       <c r="H54">
         <f t="shared" ca="1" si="6"/>
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="I54" s="1" t="s">
         <v>229</v>
@@ -4197,11 +4197,11 @@
       </c>
       <c r="G55">
         <f t="shared" ca="1" si="5"/>
-        <v>98</v>
+        <v>56</v>
       </c>
       <c r="H55">
         <f t="shared" ca="1" si="6"/>
-        <v>97</v>
+        <v>126</v>
       </c>
       <c r="I55" s="1" t="s">
         <v>230</v>
@@ -4249,11 +4249,11 @@
       </c>
       <c r="G56">
         <f t="shared" ca="1" si="5"/>
-        <v>78</v>
+        <v>47</v>
       </c>
       <c r="H56">
         <f t="shared" ca="1" si="6"/>
-        <v>124</v>
+        <v>110</v>
       </c>
       <c r="I56" s="1" t="s">
         <v>231</v>
@@ -4295,11 +4295,11 @@
       </c>
       <c r="G57">
         <f t="shared" ca="1" si="5"/>
-        <v>75</v>
+        <v>47</v>
       </c>
       <c r="H57">
         <f t="shared" ca="1" si="6"/>
-        <v>122</v>
+        <v>110</v>
       </c>
       <c r="I57" s="1" t="s">
         <v>228</v>
@@ -4341,11 +4341,11 @@
       </c>
       <c r="G58">
         <f t="shared" ca="1" si="5"/>
-        <v>90</v>
+        <v>96</v>
       </c>
       <c r="H58">
         <f t="shared" ca="1" si="6"/>
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="I58" s="1" t="s">
         <v>229</v>
@@ -4387,11 +4387,11 @@
       </c>
       <c r="G59">
         <f t="shared" ca="1" si="5"/>
-        <v>85</v>
+        <v>60</v>
       </c>
       <c r="H59">
         <f t="shared" ca="1" si="6"/>
-        <v>98</v>
+        <v>111</v>
       </c>
       <c r="I59" s="1" t="s">
         <v>228</v>
@@ -4436,11 +4436,11 @@
       </c>
       <c r="G60">
         <f t="shared" ca="1" si="5"/>
-        <v>83</v>
+        <v>88</v>
       </c>
       <c r="H60">
         <f t="shared" ca="1" si="6"/>
-        <v>109</v>
+        <v>116</v>
       </c>
       <c r="I60" s="1" t="s">
         <v>230</v>
@@ -4482,11 +4482,11 @@
       </c>
       <c r="G61">
         <f t="shared" ca="1" si="5"/>
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="H61">
         <f t="shared" ca="1" si="6"/>
-        <v>119</v>
+        <v>93</v>
       </c>
       <c r="I61" s="1" t="s">
         <v>227</v>
@@ -4529,11 +4529,11 @@
       </c>
       <c r="G62">
         <f t="shared" ca="1" si="5"/>
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="H62">
         <f t="shared" ca="1" si="6"/>
-        <v>107</v>
+        <v>113</v>
       </c>
       <c r="I62" s="1" t="s">
         <v>228</v>
@@ -4575,11 +4575,11 @@
       </c>
       <c r="G63">
         <f t="shared" ca="1" si="5"/>
-        <v>73</v>
+        <v>99</v>
       </c>
       <c r="H63">
         <f t="shared" ca="1" si="6"/>
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="I63" s="1" t="s">
         <v>227</v>
@@ -4621,11 +4621,11 @@
       </c>
       <c r="G64">
         <f t="shared" ca="1" si="5"/>
-        <v>54</v>
+        <v>61</v>
       </c>
       <c r="H64">
         <f t="shared" ca="1" si="6"/>
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="I64" s="1" t="s">
         <v>227</v>
@@ -4670,11 +4670,11 @@
       </c>
       <c r="G65">
         <f t="shared" ca="1" si="5"/>
-        <v>94</v>
+        <v>52</v>
       </c>
       <c r="H65">
         <f t="shared" ca="1" si="6"/>
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="I65" s="1" t="s">
         <v>228</v>
@@ -4716,11 +4716,11 @@
       </c>
       <c r="G66">
         <f t="shared" ref="G66:G86" ca="1" si="9">ROUND(RAND()*60+40,0)</f>
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="H66">
         <f t="shared" ref="H66:H86" ca="1" si="10">ROUND(RAND()*40+90,0)</f>
-        <v>98</v>
+        <v>107</v>
       </c>
       <c r="I66" s="1" t="s">
         <v>229</v>
@@ -4766,11 +4766,11 @@
       </c>
       <c r="G67">
         <f t="shared" ca="1" si="9"/>
-        <v>98</v>
+        <v>79</v>
       </c>
       <c r="H67">
         <f t="shared" ca="1" si="10"/>
-        <v>92</v>
+        <v>112</v>
       </c>
       <c r="I67" s="1" t="s">
         <v>230</v>
@@ -4815,11 +4815,11 @@
       </c>
       <c r="G68">
         <f t="shared" ca="1" si="9"/>
-        <v>98</v>
+        <v>53</v>
       </c>
       <c r="H68">
         <f t="shared" ca="1" si="10"/>
-        <v>109</v>
+        <v>126</v>
       </c>
       <c r="I68" s="1" t="s">
         <v>231</v>
@@ -4867,11 +4867,11 @@
       </c>
       <c r="G69">
         <f t="shared" ca="1" si="9"/>
-        <v>71</v>
+        <v>59</v>
       </c>
       <c r="H69">
         <f t="shared" ca="1" si="10"/>
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="I69" s="1" t="s">
         <v>229</v>
@@ -4916,11 +4916,11 @@
       </c>
       <c r="G70">
         <f t="shared" ca="1" si="9"/>
-        <v>88</v>
+        <v>78</v>
       </c>
       <c r="H70">
         <f t="shared" ca="1" si="10"/>
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="I70" s="1" t="s">
         <v>229</v>
@@ -4968,11 +4968,11 @@
       </c>
       <c r="G71">
         <f t="shared" ca="1" si="9"/>
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="H71">
         <f t="shared" ca="1" si="10"/>
-        <v>117</v>
+        <v>102</v>
       </c>
       <c r="I71" s="1" t="s">
         <v>229</v>
@@ -5017,11 +5017,11 @@
       </c>
       <c r="G72">
         <f t="shared" ca="1" si="9"/>
-        <v>63</v>
+        <v>42</v>
       </c>
       <c r="H72">
         <f t="shared" ca="1" si="10"/>
-        <v>126</v>
+        <v>94</v>
       </c>
       <c r="I72" s="1" t="s">
         <v>230</v>
@@ -5063,11 +5063,11 @@
       </c>
       <c r="G73">
         <f t="shared" ca="1" si="9"/>
-        <v>44</v>
+        <v>84</v>
       </c>
       <c r="H73">
         <f t="shared" ca="1" si="10"/>
-        <v>104</v>
+        <v>123</v>
       </c>
       <c r="I73" s="1" t="s">
         <v>228</v>
@@ -5112,11 +5112,11 @@
       </c>
       <c r="G74">
         <f t="shared" ca="1" si="9"/>
-        <v>43</v>
+        <v>71</v>
       </c>
       <c r="H74">
         <f t="shared" ca="1" si="10"/>
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="I74" s="1" t="s">
         <v>228</v>
@@ -5159,11 +5159,11 @@
       </c>
       <c r="G75">
         <f t="shared" ca="1" si="9"/>
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="H75">
         <f t="shared" ca="1" si="10"/>
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="I75" s="1" t="s">
         <v>227</v>
@@ -5208,11 +5208,11 @@
       </c>
       <c r="G76">
         <f t="shared" ca="1" si="9"/>
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="H76">
         <f t="shared" ca="1" si="10"/>
-        <v>96</v>
+        <v>112</v>
       </c>
       <c r="I76" s="1" t="s">
         <v>228</v>
@@ -5257,11 +5257,11 @@
       </c>
       <c r="G77">
         <f t="shared" ca="1" si="9"/>
-        <v>41</v>
+        <v>94</v>
       </c>
       <c r="H77">
         <f t="shared" ca="1" si="10"/>
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="I77" s="1" t="s">
         <v>227</v>
@@ -5306,11 +5306,11 @@
       </c>
       <c r="G78">
         <f t="shared" ca="1" si="9"/>
-        <v>57</v>
+        <v>73</v>
       </c>
       <c r="H78">
         <f t="shared" ca="1" si="10"/>
-        <v>94</v>
+        <v>113</v>
       </c>
       <c r="I78" s="1" t="s">
         <v>230</v>
@@ -5352,11 +5352,11 @@
       </c>
       <c r="G79">
         <f t="shared" ca="1" si="9"/>
-        <v>64</v>
+        <v>50</v>
       </c>
       <c r="H79">
         <f t="shared" ca="1" si="10"/>
-        <v>127</v>
+        <v>102</v>
       </c>
       <c r="I79" s="1" t="s">
         <v>230</v>
@@ -5398,11 +5398,11 @@
       </c>
       <c r="G80">
         <f t="shared" ca="1" si="9"/>
-        <v>79</v>
+        <v>99</v>
       </c>
       <c r="H80">
         <f t="shared" ca="1" si="10"/>
-        <v>120</v>
+        <v>96</v>
       </c>
       <c r="I80" s="1" t="s">
         <v>229</v>
@@ -5444,11 +5444,11 @@
       </c>
       <c r="G81">
         <f t="shared" ca="1" si="9"/>
-        <v>62</v>
+        <v>71</v>
       </c>
       <c r="H81">
         <f t="shared" ca="1" si="10"/>
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="I81" s="1" t="s">
         <v>231</v>
@@ -5493,11 +5493,11 @@
       </c>
       <c r="G82">
         <f t="shared" ca="1" si="9"/>
-        <v>45</v>
+        <v>87</v>
       </c>
       <c r="H82">
         <f t="shared" ca="1" si="10"/>
-        <v>127</v>
+        <v>94</v>
       </c>
       <c r="I82" s="1" t="s">
         <v>230</v>
@@ -5542,11 +5542,11 @@
       </c>
       <c r="G83">
         <f t="shared" ca="1" si="9"/>
-        <v>92</v>
+        <v>58</v>
       </c>
       <c r="H83">
         <f t="shared" ca="1" si="10"/>
-        <v>110</v>
+        <v>93</v>
       </c>
       <c r="I83" s="1" t="s">
         <v>231</v>
@@ -5588,11 +5588,11 @@
       </c>
       <c r="G84">
         <f t="shared" ca="1" si="9"/>
-        <v>78</v>
+        <v>87</v>
       </c>
       <c r="H84">
         <f t="shared" ca="1" si="10"/>
-        <v>104</v>
+        <v>114</v>
       </c>
       <c r="I84" s="1" t="s">
         <v>229</v>
@@ -5637,11 +5637,11 @@
       </c>
       <c r="G85">
         <f t="shared" ca="1" si="9"/>
-        <v>97</v>
+        <v>86</v>
       </c>
       <c r="H85">
         <f t="shared" ca="1" si="10"/>
-        <v>122</v>
+        <v>98</v>
       </c>
       <c r="I85" s="1" t="s">
         <v>229</v>
@@ -5683,11 +5683,11 @@
       </c>
       <c r="G86">
         <f t="shared" ca="1" si="9"/>
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="H86">
         <f t="shared" ca="1" si="10"/>
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="I86" s="1" t="s">
         <v>227</v>
@@ -6636,7 +6636,7 @@
       </c>
       <c r="D2" s="1">
         <f ca="1">(Tracker!G2+Tracker!H2)/2</f>
-        <v>100.5</v>
+        <v>103</v>
       </c>
       <c r="E2" s="1">
         <v>0.8</v>
@@ -6688,7 +6688,7 @@
       </c>
       <c r="D3" s="1">
         <f ca="1">(Tracker!G3+Tracker!H3)/2</f>
-        <v>110</v>
+        <v>100.5</v>
       </c>
       <c r="E3" s="1">
         <v>0.8</v>
@@ -6740,7 +6740,7 @@
       </c>
       <c r="D4" s="1">
         <f ca="1">(Tracker!G4+Tracker!H4)/2</f>
-        <v>73.5</v>
+        <v>89.5</v>
       </c>
       <c r="E4" s="1">
         <v>0.8</v>
@@ -6792,7 +6792,7 @@
       </c>
       <c r="D5" s="1">
         <f ca="1">(Tracker!G5+Tracker!H5)/2</f>
-        <v>104</v>
+        <v>94</v>
       </c>
       <c r="E5" s="1">
         <v>0.8</v>
@@ -6844,7 +6844,7 @@
       </c>
       <c r="D6" s="1">
         <f ca="1">(Tracker!G6+Tracker!H6)/2</f>
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="E6" s="1">
         <v>0.8</v>
@@ -6896,7 +6896,7 @@
       </c>
       <c r="D7" s="1">
         <f ca="1">(Tracker!G7+Tracker!H7)/2</f>
-        <v>97</v>
+        <v>81</v>
       </c>
       <c r="E7" s="1">
         <v>0.8</v>
@@ -6948,7 +6948,7 @@
       </c>
       <c r="D8" s="1">
         <f ca="1">(Tracker!G8+Tracker!H8)/2</f>
-        <v>86.5</v>
+        <v>72.5</v>
       </c>
       <c r="E8" s="1">
         <v>0.8</v>
@@ -7000,7 +7000,7 @@
       </c>
       <c r="D9" s="1">
         <f ca="1">(Tracker!G9+Tracker!H9)/2</f>
-        <v>102.5</v>
+        <v>88</v>
       </c>
       <c r="E9" s="1">
         <v>0.8</v>
@@ -7052,7 +7052,7 @@
       </c>
       <c r="D10" s="1">
         <f ca="1">(Tracker!G10+Tracker!H10)/2</f>
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="E10" s="1">
         <v>0.8</v>
@@ -7104,7 +7104,7 @@
       </c>
       <c r="D11" s="1">
         <f ca="1">(Tracker!G11+Tracker!H11)/2</f>
-        <v>106.5</v>
+        <v>78</v>
       </c>
       <c r="E11" s="1">
         <v>0.8</v>
@@ -7156,7 +7156,7 @@
       </c>
       <c r="D12" s="1">
         <f ca="1">(Tracker!G12+Tracker!H12)/2</f>
-        <v>83.5</v>
+        <v>94.5</v>
       </c>
       <c r="E12" s="1">
         <v>0.8</v>
@@ -7208,7 +7208,7 @@
       </c>
       <c r="D13" s="1">
         <f ca="1">(Tracker!G13+Tracker!H13)/2</f>
-        <v>101</v>
+        <v>94.5</v>
       </c>
       <c r="E13" s="1">
         <v>0.8</v>
@@ -7260,7 +7260,7 @@
       </c>
       <c r="D14" s="1">
         <f ca="1">(Tracker!G14+Tracker!H14)/2</f>
-        <v>71</v>
+        <v>100.5</v>
       </c>
       <c r="E14" s="1">
         <v>0.8</v>
@@ -7312,7 +7312,7 @@
       </c>
       <c r="D15" s="1">
         <f ca="1">(Tracker!G15+Tracker!H15)/2</f>
-        <v>95.5</v>
+        <v>101</v>
       </c>
       <c r="E15" s="1">
         <v>0.8</v>
@@ -7364,7 +7364,7 @@
       </c>
       <c r="D16" s="1">
         <f ca="1">(Tracker!G16+Tracker!H16)/2</f>
-        <v>96</v>
+        <v>108</v>
       </c>
       <c r="E16" s="1">
         <v>0.8</v>
@@ -7416,7 +7416,7 @@
       </c>
       <c r="D17" s="1">
         <f ca="1">(Tracker!G17+Tracker!H17)/2</f>
-        <v>106</v>
+        <v>104.5</v>
       </c>
       <c r="E17" s="1">
         <v>0.8</v>
@@ -7468,7 +7468,7 @@
       </c>
       <c r="D18" s="1">
         <f ca="1">(Tracker!G18+Tracker!H18)/2</f>
-        <v>71.5</v>
+        <v>66.5</v>
       </c>
       <c r="E18" s="1">
         <v>0.8</v>
@@ -7520,7 +7520,7 @@
       </c>
       <c r="D19" s="1">
         <f ca="1">(Tracker!G19+Tracker!H19)/2</f>
-        <v>94</v>
+        <v>73.5</v>
       </c>
       <c r="E19" s="1">
         <v>0.8</v>
@@ -7572,7 +7572,7 @@
       </c>
       <c r="D20" s="1">
         <f ca="1">(Tracker!G20+Tracker!H20)/2</f>
-        <v>103.5</v>
+        <v>102</v>
       </c>
       <c r="E20" s="1">
         <v>0.8</v>
@@ -7624,7 +7624,7 @@
       </c>
       <c r="D21" s="1">
         <f ca="1">(Tracker!G21+Tracker!H21)/2</f>
-        <v>103.5</v>
+        <v>78.5</v>
       </c>
       <c r="E21" s="1">
         <v>0.8</v>
@@ -7676,7 +7676,7 @@
       </c>
       <c r="D22" s="1">
         <f ca="1">(Tracker!G22+Tracker!H22)/2</f>
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="E22" s="1">
         <v>0.8</v>
@@ -7728,7 +7728,7 @@
       </c>
       <c r="D23" s="1">
         <f ca="1">(Tracker!G23+Tracker!H23)/2</f>
-        <v>82.5</v>
+        <v>94.5</v>
       </c>
       <c r="E23" s="1">
         <v>0.8</v>
@@ -7780,7 +7780,7 @@
       </c>
       <c r="D24" s="1">
         <f ca="1">(Tracker!G24+Tracker!H24)/2</f>
-        <v>87</v>
+        <v>108.5</v>
       </c>
       <c r="E24" s="1">
         <v>0.8</v>
@@ -7832,7 +7832,7 @@
       </c>
       <c r="D25" s="1">
         <f ca="1">(Tracker!G25+Tracker!H25)/2</f>
-        <v>81.5</v>
+        <v>97.5</v>
       </c>
       <c r="E25" s="1">
         <v>0.8</v>
@@ -7884,7 +7884,7 @@
       </c>
       <c r="D26" s="1">
         <f ca="1">(Tracker!G26+Tracker!H26)/2</f>
-        <v>92.5</v>
+        <v>93</v>
       </c>
       <c r="E26" s="1">
         <v>0.8</v>
@@ -7936,7 +7936,7 @@
       </c>
       <c r="D27" s="1">
         <f ca="1">(Tracker!G27+Tracker!H27)/2</f>
-        <v>75</v>
+        <v>91</v>
       </c>
       <c r="E27" s="1">
         <v>0.8</v>
@@ -7988,7 +7988,7 @@
       </c>
       <c r="D28" s="1">
         <f ca="1">(Tracker!G28+Tracker!H28)/2</f>
-        <v>99.5</v>
+        <v>98</v>
       </c>
       <c r="E28" s="1">
         <v>0.8</v>
@@ -8092,7 +8092,7 @@
       </c>
       <c r="D30" s="1">
         <f ca="1">(Tracker!G30+Tracker!H30)/2</f>
-        <v>100.5</v>
+        <v>96</v>
       </c>
       <c r="E30" s="1">
         <v>0.8</v>
@@ -8144,7 +8144,7 @@
       </c>
       <c r="D31" s="1">
         <f ca="1">(Tracker!G31+Tracker!H31)/2</f>
-        <v>85.5</v>
+        <v>95.5</v>
       </c>
       <c r="E31" s="1">
         <v>0.8</v>
@@ -8196,7 +8196,7 @@
       </c>
       <c r="D32" s="1">
         <f ca="1">(Tracker!G32+Tracker!H32)/2</f>
-        <v>85.5</v>
+        <v>82</v>
       </c>
       <c r="E32" s="1">
         <v>0.8</v>
@@ -8248,7 +8248,7 @@
       </c>
       <c r="D33" s="1">
         <f ca="1">(Tracker!G33+Tracker!H33)/2</f>
-        <v>93</v>
+        <v>65.5</v>
       </c>
       <c r="E33" s="1">
         <v>0.8</v>
@@ -8300,7 +8300,7 @@
       </c>
       <c r="D34" s="1">
         <f ca="1">(Tracker!G34+Tracker!H34)/2</f>
-        <v>96</v>
+        <v>95.5</v>
       </c>
       <c r="E34" s="1">
         <v>0.8</v>
@@ -8352,7 +8352,7 @@
       </c>
       <c r="D35" s="1">
         <f ca="1">(Tracker!G35+Tracker!H35)/2</f>
-        <v>71</v>
+        <v>78.5</v>
       </c>
       <c r="E35" s="1">
         <v>0.8</v>
@@ -8404,7 +8404,7 @@
       </c>
       <c r="D36" s="1">
         <f ca="1">(Tracker!G36+Tracker!H36)/2</f>
-        <v>97.5</v>
+        <v>80</v>
       </c>
       <c r="E36" s="1">
         <v>0.8</v>
@@ -8456,7 +8456,7 @@
       </c>
       <c r="D37" s="1">
         <f ca="1">(Tracker!G37+Tracker!H37)/2</f>
-        <v>97</v>
+        <v>69.5</v>
       </c>
       <c r="E37" s="1">
         <v>0.8</v>
@@ -8508,7 +8508,7 @@
       </c>
       <c r="D38" s="1">
         <f ca="1">(Tracker!G38+Tracker!H38)/2</f>
-        <v>95</v>
+        <v>103.5</v>
       </c>
       <c r="E38" s="1">
         <v>0.8</v>
@@ -8560,7 +8560,7 @@
       </c>
       <c r="D39" s="1">
         <f ca="1">(Tracker!G39+Tracker!H39)/2</f>
-        <v>91</v>
+        <v>82.5</v>
       </c>
       <c r="E39" s="1">
         <v>0.8</v>
@@ -8612,7 +8612,7 @@
       </c>
       <c r="D40" s="1">
         <f ca="1">(Tracker!G40+Tracker!H40)/2</f>
-        <v>80.5</v>
+        <v>79.5</v>
       </c>
       <c r="E40" s="1">
         <v>0.8</v>
@@ -8664,7 +8664,7 @@
       </c>
       <c r="D41" s="1">
         <f ca="1">(Tracker!G41+Tracker!H41)/2</f>
-        <v>74</v>
+        <v>88</v>
       </c>
       <c r="E41" s="1">
         <v>0.8</v>
@@ -8716,7 +8716,7 @@
       </c>
       <c r="D42" s="1">
         <f ca="1">(Tracker!G42+Tracker!H42)/2</f>
-        <v>75.5</v>
+        <v>99</v>
       </c>
       <c r="E42" s="1">
         <v>0.8</v>
@@ -8768,7 +8768,7 @@
       </c>
       <c r="D43" s="1">
         <f ca="1">(Tracker!G43+Tracker!H43)/2</f>
-        <v>93</v>
+        <v>94.5</v>
       </c>
       <c r="E43" s="1">
         <v>0.8</v>
@@ -8820,7 +8820,7 @@
       </c>
       <c r="D44" s="1">
         <f ca="1">(Tracker!G44+Tracker!H44)/2</f>
-        <v>106.5</v>
+        <v>84.5</v>
       </c>
       <c r="E44" s="1">
         <v>0.8</v>
@@ -8872,7 +8872,7 @@
       </c>
       <c r="D45" s="1">
         <f ca="1">(Tracker!G45+Tracker!H45)/2</f>
-        <v>87.5</v>
+        <v>89</v>
       </c>
       <c r="E45" s="1">
         <v>0.8</v>
@@ -8924,7 +8924,7 @@
       </c>
       <c r="D46" s="1">
         <f ca="1">(Tracker!G46+Tracker!H46)/2</f>
-        <v>93.5</v>
+        <v>93</v>
       </c>
       <c r="E46" s="1">
         <v>0.8</v>
@@ -8976,7 +8976,7 @@
       </c>
       <c r="D47" s="1">
         <f ca="1">(Tracker!G47+Tracker!H47)/2</f>
-        <v>75.5</v>
+        <v>88.5</v>
       </c>
       <c r="E47" s="1">
         <v>0.8</v>
@@ -9028,7 +9028,7 @@
       </c>
       <c r="D48" s="1">
         <f ca="1">(Tracker!G48+Tracker!H48)/2</f>
-        <v>92.5</v>
+        <v>99.5</v>
       </c>
       <c r="E48" s="1">
         <v>0.8</v>
@@ -9080,7 +9080,7 @@
       </c>
       <c r="D49" s="1">
         <f ca="1">(Tracker!G49+Tracker!H49)/2</f>
-        <v>84</v>
+        <v>78.5</v>
       </c>
       <c r="E49" s="1">
         <v>0.8</v>
@@ -9132,7 +9132,7 @@
       </c>
       <c r="D50" s="1">
         <f ca="1">(Tracker!G50+Tracker!H50)/2</f>
-        <v>84.5</v>
+        <v>87</v>
       </c>
       <c r="E50" s="1">
         <v>0.8</v>
@@ -9184,7 +9184,7 @@
       </c>
       <c r="D51" s="1">
         <f ca="1">(Tracker!G51+Tracker!H51)/2</f>
-        <v>96.5</v>
+        <v>103</v>
       </c>
       <c r="E51" s="1">
         <v>0.8</v>
@@ -9236,7 +9236,7 @@
       </c>
       <c r="D52" s="1">
         <f ca="1">(Tracker!G52+Tracker!H52)/2</f>
-        <v>78</v>
+        <v>84</v>
       </c>
       <c r="E52" s="1">
         <v>0.8</v>
@@ -9288,7 +9288,7 @@
       </c>
       <c r="D53" s="1">
         <f ca="1">(Tracker!G53+Tracker!H53)/2</f>
-        <v>88</v>
+        <v>96.5</v>
       </c>
       <c r="E53" s="1">
         <v>0.8</v>
@@ -9340,7 +9340,7 @@
       </c>
       <c r="D54" s="1">
         <f ca="1">(Tracker!G54+Tracker!H54)/2</f>
-        <v>91.5</v>
+        <v>98</v>
       </c>
       <c r="E54" s="1">
         <v>0.8</v>
@@ -9392,7 +9392,7 @@
       </c>
       <c r="D55" s="1">
         <f ca="1">(Tracker!G55+Tracker!H55)/2</f>
-        <v>97.5</v>
+        <v>91</v>
       </c>
       <c r="E55" s="1">
         <v>0.8</v>
@@ -9444,7 +9444,7 @@
       </c>
       <c r="D56" s="1">
         <f ca="1">(Tracker!G56+Tracker!H56)/2</f>
-        <v>101</v>
+        <v>78.5</v>
       </c>
       <c r="E56" s="1">
         <v>0.8</v>
@@ -9496,7 +9496,7 @@
       </c>
       <c r="D57" s="1">
         <f ca="1">(Tracker!G57+Tracker!H57)/2</f>
-        <v>98.5</v>
+        <v>78.5</v>
       </c>
       <c r="E57" s="1">
         <v>0.8</v>
@@ -9548,7 +9548,7 @@
       </c>
       <c r="D58" s="1">
         <f ca="1">(Tracker!G58+Tracker!H58)/2</f>
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E58" s="1">
         <v>0.8</v>
@@ -9600,7 +9600,7 @@
       </c>
       <c r="D59" s="1">
         <f ca="1">(Tracker!G59+Tracker!H59)/2</f>
-        <v>91.5</v>
+        <v>85.5</v>
       </c>
       <c r="E59" s="1">
         <v>0.8</v>
@@ -9652,7 +9652,7 @@
       </c>
       <c r="D60" s="1">
         <f ca="1">(Tracker!G60+Tracker!H60)/2</f>
-        <v>96</v>
+        <v>102</v>
       </c>
       <c r="E60" s="1">
         <v>0.8</v>
@@ -9704,7 +9704,7 @@
       </c>
       <c r="D61" s="1">
         <f ca="1">(Tracker!G61+Tracker!H61)/2</f>
-        <v>92.5</v>
+        <v>82.5</v>
       </c>
       <c r="E61" s="1">
         <v>0.8</v>
@@ -9756,7 +9756,7 @@
       </c>
       <c r="D62" s="1">
         <f ca="1">(Tracker!G62+Tracker!H62)/2</f>
-        <v>100.5</v>
+        <v>100</v>
       </c>
       <c r="E62" s="1">
         <v>0.8</v>
@@ -9808,7 +9808,7 @@
       </c>
       <c r="D63" s="1">
         <f ca="1">(Tracker!G63+Tracker!H63)/2</f>
-        <v>86.5</v>
+        <v>99</v>
       </c>
       <c r="E63" s="1">
         <v>0.8</v>
@@ -9860,7 +9860,7 @@
       </c>
       <c r="D64" s="1">
         <f ca="1">(Tracker!G64+Tracker!H64)/2</f>
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="E64" s="1">
         <v>0.8</v>
@@ -9912,7 +9912,7 @@
       </c>
       <c r="D65" s="1">
         <f ca="1">(Tracker!G65+Tracker!H65)/2</f>
-        <v>110</v>
+        <v>89.5</v>
       </c>
       <c r="E65" s="1">
         <v>0.8</v>
@@ -9964,7 +9964,7 @@
       </c>
       <c r="D66" s="1">
         <f ca="1">(Tracker!G66+Tracker!H66)/2</f>
-        <v>93.5</v>
+        <v>94</v>
       </c>
       <c r="E66" s="1">
         <v>0.8</v>
@@ -10016,7 +10016,7 @@
       </c>
       <c r="D67" s="1">
         <f ca="1">(Tracker!G67+Tracker!H67)/2</f>
-        <v>95</v>
+        <v>95.5</v>
       </c>
       <c r="E67" s="1">
         <v>0.8</v>
@@ -10068,7 +10068,7 @@
       </c>
       <c r="D68" s="1">
         <f ca="1">(Tracker!G68+Tracker!H68)/2</f>
-        <v>103.5</v>
+        <v>89.5</v>
       </c>
       <c r="E68" s="1">
         <v>0.8</v>
@@ -10120,7 +10120,7 @@
       </c>
       <c r="D69" s="1">
         <f ca="1">(Tracker!G69+Tracker!H69)/2</f>
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="E69" s="1">
         <v>0.8</v>
@@ -10172,7 +10172,7 @@
       </c>
       <c r="D70" s="1">
         <f ca="1">(Tracker!G70+Tracker!H70)/2</f>
-        <v>103</v>
+        <v>96</v>
       </c>
       <c r="E70" s="1">
         <v>0.8</v>
@@ -10224,7 +10224,7 @@
       </c>
       <c r="D71" s="1">
         <f ca="1">(Tracker!G71+Tracker!H71)/2</f>
-        <v>104</v>
+        <v>97</v>
       </c>
       <c r="E71" s="1">
         <v>0.8</v>
@@ -10276,7 +10276,7 @@
       </c>
       <c r="D72" s="1">
         <f ca="1">(Tracker!G72+Tracker!H72)/2</f>
-        <v>94.5</v>
+        <v>68</v>
       </c>
       <c r="E72" s="1">
         <v>0.8</v>
@@ -10328,7 +10328,7 @@
       </c>
       <c r="D73" s="1">
         <f ca="1">(Tracker!G73+Tracker!H73)/2</f>
-        <v>74</v>
+        <v>103.5</v>
       </c>
       <c r="E73" s="1">
         <v>0.8</v>
@@ -10380,7 +10380,7 @@
       </c>
       <c r="D74" s="1">
         <f ca="1">(Tracker!G74+Tracker!H74)/2</f>
-        <v>73</v>
+        <v>86.5</v>
       </c>
       <c r="E74" s="1">
         <v>0.8</v>
@@ -10432,7 +10432,7 @@
       </c>
       <c r="D75" s="1">
         <f ca="1">(Tracker!G75+Tracker!H75)/2</f>
-        <v>91.5</v>
+        <v>91</v>
       </c>
       <c r="E75" s="1">
         <v>0.8</v>
@@ -10484,7 +10484,7 @@
       </c>
       <c r="D76" s="1">
         <f ca="1">(Tracker!G76+Tracker!H76)/2</f>
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="E76" s="1">
         <v>0.8</v>
@@ -10536,7 +10536,7 @@
       </c>
       <c r="D77" s="1">
         <f ca="1">(Tracker!G77+Tracker!H77)/2</f>
-        <v>73.5</v>
+        <v>99.5</v>
       </c>
       <c r="E77" s="1">
         <v>0.8</v>
@@ -10588,7 +10588,7 @@
       </c>
       <c r="D78" s="1">
         <f ca="1">(Tracker!G78+Tracker!H78)/2</f>
-        <v>75.5</v>
+        <v>93</v>
       </c>
       <c r="E78" s="1">
         <v>0.8</v>
@@ -10640,7 +10640,7 @@
       </c>
       <c r="D79" s="1">
         <f ca="1">(Tracker!G79+Tracker!H79)/2</f>
-        <v>95.5</v>
+        <v>76</v>
       </c>
       <c r="E79" s="1">
         <v>0.8</v>
@@ -10692,7 +10692,7 @@
       </c>
       <c r="D80" s="1">
         <f ca="1">(Tracker!G80+Tracker!H80)/2</f>
-        <v>99.5</v>
+        <v>97.5</v>
       </c>
       <c r="E80" s="1">
         <v>0.8</v>
@@ -10744,7 +10744,7 @@
       </c>
       <c r="D81" s="1">
         <f ca="1">(Tracker!G81+Tracker!H81)/2</f>
-        <v>95.5</v>
+        <v>98.5</v>
       </c>
       <c r="E81" s="1">
         <v>0.8</v>
@@ -10796,7 +10796,7 @@
       </c>
       <c r="D82" s="1">
         <f ca="1">(Tracker!G82+Tracker!H82)/2</f>
-        <v>86</v>
+        <v>90.5</v>
       </c>
       <c r="E82" s="1">
         <v>0.8</v>
@@ -10848,7 +10848,7 @@
       </c>
       <c r="D83" s="1">
         <f ca="1">(Tracker!G83+Tracker!H83)/2</f>
-        <v>101</v>
+        <v>75.5</v>
       </c>
       <c r="E83" s="1">
         <v>0.8</v>
@@ -10900,7 +10900,7 @@
       </c>
       <c r="D84" s="1">
         <f ca="1">(Tracker!G84+Tracker!H84)/2</f>
-        <v>91</v>
+        <v>100.5</v>
       </c>
       <c r="E84" s="1">
         <v>0.8</v>
@@ -10952,7 +10952,7 @@
       </c>
       <c r="D85" s="1">
         <f ca="1">(Tracker!G85+Tracker!H85)/2</f>
-        <v>109.5</v>
+        <v>92</v>
       </c>
       <c r="E85" s="1">
         <v>0.8</v>
@@ -11004,7 +11004,7 @@
       </c>
       <c r="D86" s="1">
         <f ca="1">(Tracker!G86+Tracker!H86)/2</f>
-        <v>91.5</v>
+        <v>94</v>
       </c>
       <c r="E86" s="1">
         <v>0.8</v>

</xml_diff>